<commit_message>
Cleaned-up how blocks are defined.
</commit_message>
<xml_diff>
--- a/Research/Plush Interpreter Worksheet.xlsx
+++ b/Research/Plush Interpreter Worksheet.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarrity\Documents\Source\Repo\SOS\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9943392F-495A-46DB-B677-D3A4CC2F006D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4CD57-F6B0-4F6A-9DCD-16B14C9EFB55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{B91C377E-2224-4425-BBEB-A131CFB58DD6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Blocks Wanted" sheetId="3" r:id="rId1"/>
+    <sheet name="Block Processor" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +35,144 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Edward Garrity</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{7BA97DDD-9A91-42F5-8921-0412128E147E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Edward Garrity:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+EXEC stack before call to process instruction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{212A12C4-4C82-4B5E-98F0-8E8155A97F3D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Edward Garrity:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+How many blocks to auto reopen - 1.  State before call to process instruction.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{9374FBF2-863B-48CD-BC94-2755764F0F77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Edward Garrity
+What PopBlock() returns while processing instruction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{B25E98CA-F64E-42AD-9568-E78384D85596}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Edward Garrity:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+What is left on EXEC stack after PopBlock()</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{62E3FE6C-5D73-421E-8797-EC40C5C04FED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Edward Garrity
+What PopBlock() returns while processing instruction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{78A09EDC-25F2-448B-93D2-23F85795F62A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Edward Garrity:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+What is left on EXEC stack after PopBlock()</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="134">
   <si>
     <t>Index</t>
   </si>
@@ -1257,9 +1393,6 @@
     <t>iflte</t>
   </si>
   <si>
-    <t xml:space="preserve">exec_if </t>
-  </si>
-  <si>
     <t>{:instruction EXEC.IF :close 0}</t>
   </si>
   <si>
@@ -1267,13 +1400,43 @@
   </si>
   <si>
     <t>{:instruction 99.6 :close 1}</t>
+  </si>
+  <si>
+    <t>Blocks Wanted</t>
+  </si>
+  <si>
+    <t>Exec Stack</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>PopBlock_1()</t>
+  </si>
+  <si>
+    <t>Missing Closes 1</t>
+  </si>
+  <si>
+    <t>EXEC After Pop 1</t>
+  </si>
+  <si>
+    <t>PopBlock_2()</t>
+  </si>
+  <si>
+    <t>Missing Closes 2</t>
+  </si>
+  <si>
+    <t>EXEC After Pop 2</t>
+  </si>
+  <si>
+    <t>2.0 3 EXEC.Y 2.0 FLOAT.* 1 INTEGER.- INTEGER.DUP 0 INTEGER.&gt; EXEC.IF) EXEC.POP  1.0 FLOAT.-))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1298,6 +1461,19 @@
       <color rgb="FF009999"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1341,6 +1517,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1639,10 +1819,418 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B253EEE7-D488-46E5-8885-B234E3263687}">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="225" zoomScaleNormal="225" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B35">
+    <sortCondition ref="A2:A35"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31008868-9FAE-4AD5-8830-A05337EF61FC}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="73.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="70.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC4F167-6FF8-46B8-B986-15824370BF3F}">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
@@ -4516,7 +5104,7 @@
         <v>80</v>
       </c>
       <c r="C62">
-        <f t="shared" ref="C61:C64" si="80">C61+1</f>
+        <f t="shared" ref="C62:C64" si="80">C61+1</f>
         <v>1</v>
       </c>
       <c r="D62">
@@ -4580,7 +5168,7 @@
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C67" t="s">
         <v>15</v>
@@ -4641,7 +5229,7 @@
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -4649,7 +5237,7 @@
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C69">
         <f t="shared" ref="C69" si="86">C68+1</f>
@@ -4665,308 +5253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B253EEE7-D488-46E5-8885-B234E3263687}">
-  <dimension ref="A1:B35"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="225" zoomScaleNormal="225" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>117</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>116</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B35">
-    <sortCondition ref="A2:A35"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE9F5D3-2FDC-4767-A2E6-FE1C44D6AF85}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -5076,30 +5363,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31008868-9FAE-4AD5-8830-A05337EF61FC}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView zoomScale="313" zoomScaleNormal="313" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1">
-        <v>123</v>
-      </c>
-      <c r="C1">
-        <v>99.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Moved CodeAtom and ExecAtom into Genome class.  Added length(), split(), and pop() methods in Genome to handle Plush code objects.
</commit_message>
<xml_diff>
--- a/Research/Plush Interpreter Worksheet.xlsx
+++ b/Research/Plush Interpreter Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarrity\Documents\Source\Repo\SOS\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CA48E6-38AA-4DEC-9C80-44791D5A036D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D817C3-EC6A-434F-B3F0-EBDBD8B64D29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{B91C377E-2224-4425-BBEB-A131CFB58DD6}"/>
   </bookViews>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="144">
   <si>
     <t>Index</t>
   </si>
@@ -1451,28 +1451,16 @@
     <t>{:instruction 2.1 :close 1}</t>
   </si>
   <si>
-    <t>{:instruction 3.0 :close 2}</t>
-  </si>
-  <si>
-    <t>{:instruction 1 :close 1}</t>
-  </si>
-  <si>
-    <t>{:instruction CODE.NTHCDR :close 1}</t>
-  </si>
-  <si>
-    <t>block_number</t>
-  </si>
-  <si>
     <t>wanted_stack</t>
   </si>
   <si>
     <t>Hidden</t>
   </si>
   <si>
-    <t>()(</t>
-  </si>
-  <si>
-    <t>0,1</t>
+    <t>item_number</t>
+  </si>
+  <si>
+    <t>-1,1</t>
   </si>
 </sst>
 </file>
@@ -1539,13 +1527,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2270,10 +2261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C94DFA-6C6F-4651-8240-87F9ED788928}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2289,13 +2280,13 @@
         <v>85</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2317,8 +2308,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>147</v>
+      <c r="D3" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,8 +2319,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>147</v>
+      <c r="D4" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2339,8 +2330,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>147</v>
+      <c r="D5" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2351,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2359,63 +2350,21 @@
         <v>138</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>139</v>
       </c>
-      <c r="B8" t="s">
-        <v>126</v>
-      </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing bug with CODE.SUBST.
</commit_message>
<xml_diff>
--- a/Research/Plush Interpreter Worksheet.xlsx
+++ b/Research/Plush Interpreter Worksheet.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarrity\Documents\Source\Repo\SOS\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D817C3-EC6A-434F-B3F0-EBDBD8B64D29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3220ABB8-3B3A-4931-84EA-1BC3D23DD131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{B91C377E-2224-4425-BBEB-A131CFB58DD6}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{B91C377E-2224-4425-BBEB-A131CFB58DD6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blocks Wanted" sheetId="3" r:id="rId1"/>
-    <sheet name="Block Processor" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Subst" sheetId="6" r:id="rId1"/>
+    <sheet name="Blocks Wanted" sheetId="3" r:id="rId2"/>
+    <sheet name="Block Processor" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -173,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="154">
   <si>
     <t>Index</t>
   </si>
@@ -1461,6 +1462,36 @@
   </si>
   <si>
     <t>-1,1</t>
+  </si>
+  <si>
+    <t>{:instruction EXEC.NOOP_OPEN_PAREN :close 0}\</t>
+  </si>
+  <si>
+    <t>{:instruction EXEC.DO*RANGE :close 0}\</t>
+  </si>
+  <si>
+    <t>{:instruction FLOAT.+ :close 2}\</t>
+  </si>
+  <si>
+    <t>{:instruction FLOAT.- :close 1}\</t>
+  </si>
+  <si>
+    <t>{:instruction FLOAT.+ :close 1}\</t>
+  </si>
+  <si>
+    <t>{:instruction CODE.SUBST :close 0}\</t>
+  </si>
+  <si>
+    <t>extra_blocks</t>
+  </si>
+  <si>
+    <t>closing</t>
+  </si>
+  <si>
+    <t>wanted_blocks</t>
+  </si>
+  <si>
+    <t>0, 1</t>
   </si>
 </sst>
 </file>
@@ -1852,6 +1883,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7015191-2302-41E8-813B-970F1634A532}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B253EEE7-D488-46E5-8885-B234E3263687}">
   <dimension ref="A1:B35"/>
   <sheetViews>
@@ -2150,7 +2317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31008868-9FAE-4AD5-8830-A05337EF61FC}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -2259,11 +2426,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C94DFA-6C6F-4651-8240-87F9ED788928}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2372,7 +2539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC4F167-6FF8-46B8-B986-15824370BF3F}">
   <dimension ref="A1:S69"/>
   <sheetViews>
@@ -5399,7 +5566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE9F5D3-2FDC-4767-A2E6-FE1C44D6AF85}">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>